<commit_message>
New case file based on literature validation
</commit_message>
<xml_diff>
--- a/stockwellExample/RawInputData/A-Phase-1.xlsx
+++ b/stockwellExample/RawInputData/A-Phase-1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttcd\Documents\MATLAB\PetriNetSimulate\sophisticatedExample\RawInputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttcd\Documents\MATLAB\PetriNetSimulate\stockwellExample\RawInputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C2ED18-78F9-48C3-84D5-859437DD9756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010F67B0-C9B0-4084-8190-293C771920E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E6BF008F-5C6C-4F49-B7F4-2457C7664101}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6BF008F-5C6C-4F49-B7F4-2457C7664101}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -172,9 +172,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -212,7 +212,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -318,7 +318,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -460,7 +460,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -470,19 +470,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAB0E9C-5A6F-0C40-BF0F-F44C8FBE3B7B}">
   <dimension ref="E1:AG24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="63" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Z6" sqref="Z6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="2.83203125" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" customWidth="1"/>
-    <col min="6" max="6" width="7.1640625" customWidth="1"/>
-    <col min="7" max="36" width="3.83203125" customWidth="1"/>
+    <col min="1" max="4" width="2.875" customWidth="1"/>
+    <col min="5" max="5" width="18.125" customWidth="1"/>
+    <col min="6" max="6" width="7.125" customWidth="1"/>
+    <col min="7" max="36" width="3.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:33" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="5:33" ht="166.5" x14ac:dyDescent="0.25">
       <c r="G1" s="7" t="s">
         <v>0</v>
       </c>
@@ -504,100 +504,56 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="5:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="5:33" x14ac:dyDescent="0.25">
       <c r="G2" s="1">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H2" s="1">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I2" s="1">
+        <v>103</v>
+      </c>
+      <c r="J2" s="1">
+        <v>104</v>
+      </c>
+      <c r="K2" s="1">
+        <v>105</v>
+      </c>
+      <c r="L2" s="1">
+        <v>106</v>
+      </c>
+      <c r="Y2" s="5">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="5">
         <v>101</v>
       </c>
-      <c r="J2" s="1">
-        <v>102</v>
-      </c>
-      <c r="K2" s="1">
-        <v>103</v>
-      </c>
-      <c r="L2" s="1">
-        <v>104</v>
-      </c>
-      <c r="M2" s="1">
-        <v>105</v>
-      </c>
-      <c r="N2" s="1">
-        <v>106</v>
-      </c>
-      <c r="O2" s="1">
-        <v>107</v>
-      </c>
-      <c r="P2" s="1">
-        <v>108</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>109</v>
-      </c>
-      <c r="R2" s="1">
-        <v>110</v>
-      </c>
-      <c r="Y2" s="5">
-        <v>48</v>
-      </c>
-      <c r="Z2" s="5">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="5:33" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="5:33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="2">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="G3" s="2">
         <v>-1</v>
       </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0</v>
-      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
       <c r="L3" s="2">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0</v>
-      </c>
-      <c r="O3" s="2">
-        <v>0</v>
-      </c>
-      <c r="P3" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>0</v>
-      </c>
-      <c r="R3" s="2">
         <v>1</v>
       </c>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="5">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="Z3" s="5">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
@@ -607,51 +563,25 @@
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
     </row>
-    <row r="4" spans="5:33" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="5:33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="8"/>
       <c r="F4" s="2">
-        <v>53</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="G4" s="2"/>
       <c r="H4" s="2">
         <v>-1</v>
       </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2">
         <v>1</v>
-      </c>
-      <c r="K4" s="2">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2">
-        <v>0</v>
-      </c>
-      <c r="N4" s="2">
-        <v>0</v>
-      </c>
-      <c r="O4" s="2">
-        <v>0</v>
-      </c>
-      <c r="P4" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>0</v>
-      </c>
-      <c r="R4" s="2">
-        <v>0</v>
       </c>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="5">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="Z4" s="5">
         <v>103</v>
@@ -664,54 +594,28 @@
       <c r="AF4" s="2"/>
       <c r="AG4" s="2"/>
     </row>
-    <row r="5" spans="5:33" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="5:33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" s="8"/>
       <c r="F5" s="2">
-        <v>54</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
       <c r="I5" s="2">
         <v>-1</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="2"/>
+      <c r="K5" s="2">
         <v>1</v>
       </c>
-      <c r="K5" s="2">
-        <v>0</v>
-      </c>
-      <c r="L5" s="2">
-        <v>0</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0</v>
-      </c>
-      <c r="O5" s="2">
-        <v>0</v>
-      </c>
-      <c r="P5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>0</v>
-      </c>
-      <c r="R5" s="2">
-        <v>0</v>
-      </c>
+      <c r="L5" s="2"/>
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="5">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="Z5" s="5">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
@@ -721,55 +625,25 @@
       <c r="AF5" s="2"/>
       <c r="AG5" s="2"/>
     </row>
-    <row r="6" spans="5:33" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="5:33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E6" s="8"/>
       <c r="F6" s="2">
-        <v>55</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
       <c r="J6" s="2">
         <v>-1</v>
       </c>
       <c r="K6" s="2">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2">
         <v>1</v>
       </c>
-      <c r="M6" s="2">
-        <v>0</v>
-      </c>
-      <c r="N6" s="2">
-        <v>0</v>
-      </c>
-      <c r="O6" s="2">
-        <v>0</v>
-      </c>
-      <c r="P6" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>0</v>
-      </c>
-      <c r="R6" s="2">
-        <v>0</v>
-      </c>
+      <c r="L6" s="2"/>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
-      <c r="Y6" s="5">
-        <v>52</v>
-      </c>
-      <c r="Z6" s="5">
-        <v>101</v>
-      </c>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
@@ -778,55 +652,25 @@
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
     </row>
-    <row r="7" spans="5:33" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="5:33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E7" s="8"/>
       <c r="F7" s="2">
-        <v>56</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
       <c r="K7" s="2">
         <v>-1</v>
       </c>
       <c r="L7" s="2">
         <v>1</v>
       </c>
-      <c r="M7" s="2">
-        <v>0</v>
-      </c>
-      <c r="N7" s="2">
-        <v>0</v>
-      </c>
-      <c r="O7" s="2">
-        <v>0</v>
-      </c>
-      <c r="P7" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>0</v>
-      </c>
-      <c r="R7" s="2">
-        <v>0</v>
-      </c>
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
-      <c r="Y7" s="6">
-        <v>53</v>
-      </c>
-      <c r="Z7" s="6">
-        <v>99</v>
-      </c>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
@@ -835,47 +679,20 @@
       <c r="AF7" s="2"/>
       <c r="AG7" s="2"/>
     </row>
-    <row r="8" spans="5:33" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="5:33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E8" s="8"/>
-      <c r="F8" s="2">
-        <v>57</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0</v>
-      </c>
-      <c r="K8" s="2">
-        <v>0</v>
-      </c>
-      <c r="L8" s="2">
-        <v>-1</v>
-      </c>
-      <c r="M8" s="2">
-        <v>0</v>
-      </c>
-      <c r="N8" s="2">
-        <v>0</v>
-      </c>
-      <c r="O8" s="2">
-        <v>0</v>
-      </c>
-      <c r="P8" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>0</v>
-      </c>
-      <c r="R8" s="2">
-        <v>1</v>
-      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
@@ -888,47 +705,20 @@
       <c r="AF8" s="2"/>
       <c r="AG8" s="2"/>
     </row>
-    <row r="9" spans="5:33" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="5:33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E9" s="8"/>
-      <c r="F9" s="2">
-        <v>58</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0</v>
-      </c>
-      <c r="K9" s="2">
-        <v>0</v>
-      </c>
-      <c r="L9" s="2">
-        <v>0</v>
-      </c>
-      <c r="M9" s="2">
-        <v>-1</v>
-      </c>
-      <c r="N9" s="2">
-        <v>-1</v>
-      </c>
-      <c r="O9" s="2">
-        <v>0</v>
-      </c>
-      <c r="P9" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>1</v>
-      </c>
-      <c r="R9" s="2">
-        <v>0</v>
-      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
@@ -941,47 +731,20 @@
       <c r="AF9" s="2"/>
       <c r="AG9" s="2"/>
     </row>
-    <row r="10" spans="5:33" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="5:33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E10" s="8"/>
-      <c r="F10" s="2">
-        <v>59</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2">
-        <v>0</v>
-      </c>
-      <c r="L10" s="2">
-        <v>0</v>
-      </c>
-      <c r="M10" s="2">
-        <v>0</v>
-      </c>
-      <c r="N10" s="2">
-        <v>0</v>
-      </c>
-      <c r="O10" s="2">
-        <v>-1</v>
-      </c>
-      <c r="P10" s="2">
-        <v>-1</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>1</v>
-      </c>
-      <c r="R10" s="2">
-        <v>0</v>
-      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
@@ -994,47 +757,20 @@
       <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
     </row>
-    <row r="11" spans="5:33" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="5:33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E11" s="8"/>
-      <c r="F11" s="2">
-        <v>60</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0</v>
-      </c>
-      <c r="K11" s="2">
-        <v>0</v>
-      </c>
-      <c r="L11" s="2">
-        <v>0</v>
-      </c>
-      <c r="M11" s="2">
-        <v>0</v>
-      </c>
-      <c r="N11" s="2">
-        <v>0</v>
-      </c>
-      <c r="O11" s="2">
-        <v>0</v>
-      </c>
-      <c r="P11" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>-1</v>
-      </c>
-      <c r="R11" s="2">
-        <v>1</v>
-      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
@@ -1047,7 +783,7 @@
       <c r="AF11" s="2"/>
       <c r="AG11" s="2"/>
     </row>
-    <row r="12" spans="5:33" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="5:33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E12" s="8"/>
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
@@ -1061,7 +797,7 @@
       <c r="AF12" s="2"/>
       <c r="AG12" s="2"/>
     </row>
-    <row r="13" spans="5:33" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="5:33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E13" s="8"/>
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
@@ -1075,7 +811,7 @@
       <c r="AF13" s="2"/>
       <c r="AG13" s="2"/>
     </row>
-    <row r="14" spans="5:33" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="5:33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E14" s="8"/>
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
@@ -1089,7 +825,7 @@
       <c r="AF14" s="2"/>
       <c r="AG14" s="2"/>
     </row>
-    <row r="15" spans="5:33" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="5:33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E15" s="8"/>
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
@@ -1103,16 +839,16 @@
       <c r="AF15" s="2"/>
       <c r="AG15" s="2"/>
     </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G18" s="3"/>
     </row>
-    <row r="22" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H24" s="2"/>
     </row>
   </sheetData>
@@ -1138,6 +874,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007EAC084835D24746A54539AB1A640141" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4ffd6c716aa37c768830efd8a6f66906">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="db6488ae-1ae9-46d0-aa9c-9ac0f238754f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd3435f0d87b5839f740039772a9ff86" ns2:_="">
     <xsd:import namespace="db6488ae-1ae9-46d0-aa9c-9ac0f238754f"/>
@@ -1321,12 +1063,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF387451-9C43-4878-8CD8-AC44434AD390}">
   <ds:schemaRefs>
@@ -1336,6 +1072,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5B3618C-B144-4565-9E3E-0F842207522B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAAD9EA9-EEA7-4F73-A048-DA11FD7FFA3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1351,13 +1096,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5B3618C-B144-4565-9E3E-0F842207522B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>